<commit_message>
merged vacancies and statistics scripts
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Статистика по годам" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Статистика по городам" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Статистика по годам" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Статистика по городам" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,9 +445,9 @@
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="29" customWidth="1" min="3" max="3"/>
+    <col width="32" customWidth="1" min="3" max="3"/>
     <col width="21" customWidth="1" min="4" max="4"/>
-    <col width="32" customWidth="1" min="5" max="5"/>
+    <col width="35" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -463,7 +463,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Средняя зарплата - Аналитик</t>
+          <t>Средняя зарплата - Программист</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -473,280 +473,25 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Количество вакансий - Аналитик</t>
+          <t>Количество вакансий - Программист</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>2007</v>
+        <v>2022</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>38916</v>
+        <v>112106</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>40641</v>
+        <v>2946</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2196</v>
+        <v>108090</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>2008</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>43646</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>48428</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>17549</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>2009</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>42492</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>48109</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>17709</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>2010</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>43846</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>49577</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>29093</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>2011</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>47451</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>52794</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>36700</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>2012</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>48243</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>58341</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>44153</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>2013</v>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>51510</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>57004</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>59954</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>2014</v>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>50658</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>58768</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>66837</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>2015</v>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>52696</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>53326</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>70039</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>2016</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>62675</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>54236</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>75145</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
-        <v>2017</v>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>60935</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>56558</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>82823</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>1201</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
-        <v>2018</v>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>58335</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>61080</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>131701</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>1578</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="n">
-        <v>2019</v>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>69467</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>71288</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>115086</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>1482</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
-        <v>2020</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>73431</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>80145</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>102243</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>1349</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
-        <v>2021</v>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>82690</v>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>87473</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>57623</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="n">
-        <v>2022</v>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>91795</v>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>91340</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>18294</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>305</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -805,7 +550,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>76970</v>
+        <v>144297</v>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
@@ -813,43 +558,43 @@
         </is>
       </c>
       <c r="E2" s="4" t="n">
-        <v>0.3246</v>
+        <v>0.2332</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
+          <t>Казань</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>114143</v>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
           <t>Санкт-Петербург</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>65286</v>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Санкт-Петербург</t>
-        </is>
-      </c>
       <c r="E3" s="4" t="n">
-        <v>0.1197</v>
+        <v>0.1039</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Новосибирск</t>
+          <t>Санкт-Петербург</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>62254</v>
+        <v>112632</v>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Новосибирск</t>
+          <t>Алматы</t>
         </is>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0.0271</v>
+        <v>0.0282</v>
       </c>
     </row>
     <row r="5">
@@ -859,123 +604,123 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>60962</v>
+        <v>97283</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>Казань</t>
+          <t>Новосибирск</t>
         </is>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0.0237</v>
+        <v>0.0268</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
+          <t>Пермь</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>91220</v>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
           <t>Казань</t>
         </is>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>52580</v>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>Нижний Новгород</t>
-        </is>
-      </c>
       <c r="E6" s="4" t="n">
-        <v>0.0232</v>
+        <v>0.0234</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Краснодар</t>
+          <t>Новосибирск</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>51644</v>
+        <v>83421</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>Ростов-на-Дону</t>
+          <t>Екатеринбург</t>
         </is>
       </c>
       <c r="E7" s="4" t="n">
-        <v>0.0209</v>
+        <v>0.0231</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Челябинск</t>
+          <t>Ростов-на-Дону</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>51265</v>
+        <v>83308</v>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>Екатеринбург</t>
+          <t>Краснодар</t>
         </is>
       </c>
       <c r="E8" s="4" t="n">
-        <v>0.0207</v>
+        <v>0.0217</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Самара</t>
+          <t>Уфа</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>50994</v>
+        <v>83173</v>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>Краснодар</t>
+          <t>Минск</t>
         </is>
       </c>
       <c r="E9" s="4" t="n">
-        <v>0.0185</v>
+        <v>0.0204</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Пермь</t>
+          <t>Воронеж</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>48089</v>
+        <v>83054</v>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>Самара</t>
+          <t>Ростов-на-Дону</t>
         </is>
       </c>
       <c r="E10" s="4" t="n">
-        <v>0.0143</v>
+        <v>0.0187</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
+          <t>Краснодар</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>79239</v>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
           <t>Нижний Новгород</t>
         </is>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>47662</v>
-      </c>
-      <c r="D11" s="2" t="inlineStr">
-        <is>
-          <t>Воронеж</t>
-        </is>
-      </c>
       <c r="E11" s="4" t="n">
-        <v>0.0141</v>
+        <v>0.0156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>